<commit_message>
Updated BOM / Removed extra one
</commit_message>
<xml_diff>
--- a/Senior Design Financial Spreadsheet.xlsx
+++ b/Senior Design Financial Spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abbybright/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rynoe\Desktop\School\Fall 2022 Semester\4 - Principles of Electrical and Computer Eng Design\3 - Project Code\Senior-Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C5E9F5-651B-124E-89EB-80415BE6A9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C701F9-1BEA-46D2-BBEF-E5C2BBF97240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" xr2:uid="{8178A0F5-9EBE-431C-92C4-B6AF08CBCA09}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8178A0F5-9EBE-431C-92C4-B6AF08CBCA09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>Expenses</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>Detachable Connector</t>
+  </si>
+  <si>
+    <t>Akaline 9V Battery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch Toggle </t>
   </si>
 </sst>
 </file>
@@ -169,15 +175,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -495,96 +501,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25DB686C-FDF5-4CAE-BA07-B9A70B77A3FB}">
   <dimension ref="B2:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="4" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4" t="s">
+      <c r="G3" s="7"/>
+      <c r="H3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4" t="s">
+      <c r="I3" s="7"/>
+      <c r="J3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4" t="s">
+      <c r="K3" s="7"/>
+      <c r="L3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B4" s="6" t="s">
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -608,7 +614,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>25</v>
       </c>
@@ -632,7 +638,7 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>22</v>
       </c>
@@ -656,7 +662,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -680,8 +686,22 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="F9" s="2"/>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.95</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -690,8 +710,22 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="F10" s="2"/>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2.5</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -700,7 +734,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -710,7 +744,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -720,7 +754,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -730,7 +764,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -740,7 +774,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -750,7 +784,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -760,7 +794,7 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -770,7 +804,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -780,7 +814,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -790,7 +824,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -800,7 +834,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>9</v>
       </c>
@@ -814,7 +848,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="E22" s="1"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -825,7 +859,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="E23" s="1"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -836,7 +870,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="E24" s="1"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -847,14 +881,14 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D25" s="5"/>
-      <c r="E25" s="7" t="s">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D25" s="4"/>
+      <c r="E25" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F25" s="2">
         <f>SUM(F5:F24)</f>
-        <v>15.85</v>
+        <v>20.3</v>
       </c>
       <c r="G25" s="2">
         <f t="shared" ref="G25:M25" si="0">SUM(G5:G24)</f>
@@ -885,23 +919,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D26" s="5"/>
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D27" s="5"/>
-      <c r="E27" s="5" t="s">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D26" s="4"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D27" s="4"/>
+      <c r="E27" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="3">
         <f>SUM(F25:G25)</f>
-        <v>15.85</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D28" s="5"/>
-      <c r="E28" s="5" t="s">
+        <v>20.3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D28" s="4"/>
+      <c r="E28" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F28" s="3">
@@ -909,9 +943,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D29" s="5"/>
-      <c r="E29" s="7" t="s">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D29" s="4"/>
+      <c r="E29" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F29" s="3">
@@ -919,9 +953,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D30" s="5"/>
-      <c r="E30" s="7" t="s">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D30" s="4"/>
+      <c r="E30" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="3">

</xml_diff>